<commit_message>
corrected reference designators, some were FLMA.  Added controllers to integration csv
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI03FLMB_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GI03FLMB_00002.xlsx
@@ -22,12 +22,12 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="132">
   <si>
     <t>Ref Des</t>
   </si>
@@ -291,75 +291,6 @@
     <t>GI03FLMB-RIM01-02-ADCPSL007</t>
   </si>
   <si>
-    <t>GI03FLMB-RIM01-02-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GI03FLMB-FMS01-01-SIOENG000</t>
-  </si>
-  <si>
-    <t>GI03FLMB-FMM01-01-SIOENG000</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG060</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG061</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG062</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG063</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG064</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG065</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG066</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG067</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOG068</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOH071</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOH070</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-02-CTDMOH069</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-CTDMOH000</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-CTDMOH700</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-CTDMOH400</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-CTDMOH100</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-VELPTB000</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-VELPTB700</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-VELPTB400</t>
-  </si>
-  <si>
-    <t>GI03FLMA-RI000-00-VELPTB100</t>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -451,6 +382,66 @@
   </si>
   <si>
     <t>OL000026</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG060</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG061</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG062</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG063</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG064</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG065</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG066</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG067</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOG068</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOH069</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOH070</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RIM01-02-CTDMOH071</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-CTDMOH000</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-CTDMOH700</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-CTDMOH400</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-CTDMOH100</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-VELPTB000</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-VELPTB700</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-VELPTB400</t>
+  </si>
+  <si>
+    <t>GI03FLMB-RI000-00-VELPTB100</t>
   </si>
 </sst>
 </file>
@@ -958,7 +949,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1093,9 +1084,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1627,7 +1615,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1650,47 +1638,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="33" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="53" t="s">
+      <c r="A1" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="53"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:14" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>73</v>
@@ -1743,11 +1731,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q131"/>
+  <dimension ref="A1:Q134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G141" sqref="G141"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1768,12 +1756,12 @@
     <col min="18" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>104</v>
+      <c r="B1" s="50" t="s">
+        <v>81</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1</v>
@@ -1781,16 +1769,16 @@
       <c r="D1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="51" t="s">
-        <v>105</v>
+      <c r="E1" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="51" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="14" t="s">
@@ -1803,7 +1791,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1820,12 +1808,12 @@
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>48</v>
@@ -1834,7 +1822,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F3" s="19">
         <v>1299</v>
@@ -1857,12 +1845,12 @@
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>48</v>
@@ -1871,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F4" s="32">
         <v>1299</v>
@@ -1892,12 +1880,12 @@
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>48</v>
@@ -1906,7 +1894,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F5" s="32">
         <v>1299</v>
@@ -1925,12 +1913,12 @@
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>48</v>
@@ -1939,7 +1927,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F6" s="32">
         <v>1299</v>
@@ -1958,12 +1946,12 @@
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>48</v>
@@ -1972,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F7" s="32">
         <v>1299</v>
@@ -1991,12 +1979,12 @@
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>48</v>
@@ -2005,7 +1993,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F8" s="32">
         <v>1299</v>
@@ -2024,12 +2012,12 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>48</v>
@@ -2038,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F9" s="32">
         <v>1299</v>
@@ -2059,12 +2047,12 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>48</v>
@@ -2073,7 +2061,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F10" s="32">
         <v>1299</v>
@@ -2094,12 +2082,12 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>48</v>
@@ -2108,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F11" s="32">
         <v>1299</v>
@@ -2124,19 +2112,17 @@
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="8"/>
+      <c r="L11" s="19"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>48</v>
@@ -2145,7 +2131,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F12" s="32">
         <v>1299</v>
@@ -2165,11 +2151,8 @@
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="29"/>
@@ -2185,16 +2168,13 @@
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
-      <c r="P13" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>48</v>
@@ -2203,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>49</v>
@@ -2226,12 +2206,12 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>48</v>
@@ -2240,7 +2220,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>49</v>
@@ -2259,12 +2239,12 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>48</v>
@@ -2273,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>49</v>
@@ -2297,7 +2277,7 @@
         <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>48</v>
@@ -2306,7 +2286,7 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F17" s="32" t="s">
         <v>49</v>
@@ -2330,7 +2310,7 @@
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>48</v>
@@ -2339,7 +2319,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>49</v>
@@ -2357,14 +2337,13 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="Q18" s="18"/>
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C19" s="29" t="s">
         <v>48</v>
@@ -2373,7 +2352,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>49</v>
@@ -2397,7 +2376,7 @@
         <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>48</v>
@@ -2406,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>49</v>
@@ -2449,7 +2428,7 @@
         <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>48</v>
@@ -2458,7 +2437,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="F22" s="19">
         <v>466</v>
@@ -2486,7 +2465,7 @@
         <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C23" s="29" t="s">
         <v>48</v>
@@ -2495,7 +2474,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="F23" s="32">
         <v>466</v>
@@ -2521,7 +2500,7 @@
         <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C24" s="29" t="s">
         <v>48</v>
@@ -2530,7 +2509,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="F24" s="32">
         <v>466</v>
@@ -2571,7 +2550,7 @@
         <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>48</v>
@@ -2580,7 +2559,7 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F26" s="19">
         <v>23381</v>
@@ -2608,7 +2587,7 @@
         <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>48</v>
@@ -2617,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F27" s="32">
         <v>23381</v>
@@ -2641,7 +2620,7 @@
         <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>48</v>
@@ -2650,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F28" s="32">
         <v>23381</v>
@@ -2674,7 +2653,7 @@
         <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>48</v>
@@ -2683,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F29" s="32">
         <v>23381</v>
@@ -2707,7 +2686,7 @@
         <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>48</v>
@@ -2716,7 +2695,7 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F30" s="32">
         <v>23381</v>
@@ -2740,7 +2719,7 @@
         <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C31" s="29" t="s">
         <v>48</v>
@@ -2749,7 +2728,7 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F31" s="32">
         <v>23381</v>
@@ -2773,7 +2752,7 @@
         <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C32" s="29" t="s">
         <v>48</v>
@@ -2782,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F32" s="32">
         <v>23381</v>
@@ -2807,7 +2786,7 @@
         <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>48</v>
@@ -2816,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F33" s="32">
         <v>23381</v>
@@ -2841,7 +2820,7 @@
         <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>48</v>
@@ -2850,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F34" s="32">
         <v>23381</v>
@@ -2887,11 +2866,11 @@
       <c r="O35" s="16"/>
     </row>
     <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>84</v>
+      <c r="A36" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>48</v>
@@ -2900,7 +2879,7 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>50</v>
@@ -2924,11 +2903,11 @@
       <c r="O36" s="16"/>
     </row>
     <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>84</v>
+      <c r="A37" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>48</v>
@@ -2937,7 +2916,7 @@
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F37" s="32" t="s">
         <v>50</v>
@@ -2957,11 +2936,11 @@
       <c r="O37" s="16"/>
     </row>
     <row r="38" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>84</v>
+      <c r="A38" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C38" s="29" t="s">
         <v>48</v>
@@ -2970,7 +2949,7 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F38" s="32" t="s">
         <v>50</v>
@@ -2990,11 +2969,11 @@
       <c r="O38" s="16"/>
     </row>
     <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
-        <v>84</v>
+      <c r="A39" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C39" s="29" t="s">
         <v>48</v>
@@ -3003,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F39" s="32" t="s">
         <v>50</v>
@@ -3040,11 +3019,11 @@
       <c r="O40" s="16"/>
     </row>
     <row r="41" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>85</v>
+      <c r="A41" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>48</v>
@@ -3053,7 +3032,7 @@
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="F41" s="19" t="s">
         <v>51</v>
@@ -3077,11 +3056,11 @@
       <c r="O41" s="16"/>
     </row>
     <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>85</v>
+      <c r="A42" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C42" s="29" t="s">
         <v>48</v>
@@ -3090,7 +3069,7 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="F42" s="32" t="s">
         <v>51</v>
@@ -3110,11 +3089,11 @@
       <c r="O42" s="16"/>
     </row>
     <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>85</v>
+      <c r="A43" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C43" s="29" t="s">
         <v>48</v>
@@ -3123,7 +3102,7 @@
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="F43" s="32" t="s">
         <v>51</v>
@@ -3143,11 +3122,11 @@
       <c r="O43" s="16"/>
     </row>
     <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>85</v>
+      <c r="A44" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C44" s="29" t="s">
         <v>48</v>
@@ -3156,7 +3135,7 @@
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="F44" s="32" t="s">
         <v>51</v>
@@ -3193,11 +3172,11 @@
       <c r="O45" s="16"/>
     </row>
     <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>86</v>
+      <c r="A46" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C46" s="30" t="s">
         <v>48</v>
@@ -3206,7 +3185,7 @@
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>52</v>
@@ -3230,11 +3209,11 @@
       <c r="O46" s="16"/>
     </row>
     <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>86</v>
+      <c r="A47" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C47" s="29" t="s">
         <v>48</v>
@@ -3243,7 +3222,7 @@
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="F47" s="32" t="s">
         <v>52</v>
@@ -3263,11 +3242,11 @@
       <c r="O47" s="16"/>
     </row>
     <row r="48" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
-        <v>86</v>
+      <c r="A48" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C48" s="29" t="s">
         <v>48</v>
@@ -3276,7 +3255,7 @@
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="F48" s="32" t="s">
         <v>52</v>
@@ -3296,11 +3275,11 @@
       <c r="O48" s="16"/>
     </row>
     <row r="49" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>86</v>
+      <c r="A49" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C49" s="29" t="s">
         <v>48</v>
@@ -3309,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="F49" s="32" t="s">
         <v>52</v>
@@ -3346,11 +3325,11 @@
       <c r="O50" s="16"/>
     </row>
     <row r="51" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>87</v>
+      <c r="A51" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C51" s="30" t="s">
         <v>48</v>
@@ -3359,7 +3338,7 @@
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F51" s="19" t="s">
         <v>53</v>
@@ -3383,11 +3362,11 @@
       <c r="O51" s="16"/>
     </row>
     <row r="52" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
-        <v>87</v>
+      <c r="A52" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>48</v>
@@ -3396,7 +3375,7 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F52" s="32" t="s">
         <v>53</v>
@@ -3416,11 +3395,11 @@
       <c r="O52" s="16"/>
     </row>
     <row r="53" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
-        <v>87</v>
+      <c r="A53" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C53" s="29" t="s">
         <v>48</v>
@@ -3429,7 +3408,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F53" s="32" t="s">
         <v>53</v>
@@ -3449,11 +3428,11 @@
       <c r="O53" s="16"/>
     </row>
     <row r="54" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
-        <v>87</v>
+      <c r="A54" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C54" s="29" t="s">
         <v>48</v>
@@ -3462,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F54" s="32" t="s">
         <v>53</v>
@@ -3499,11 +3478,11 @@
       <c r="O55" s="16"/>
     </row>
     <row r="56" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
-        <v>88</v>
+      <c r="A56" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C56" s="30" t="s">
         <v>48</v>
@@ -3512,7 +3491,7 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F56" s="19" t="s">
         <v>54</v>
@@ -3536,11 +3515,11 @@
       <c r="O56" s="16"/>
     </row>
     <row r="57" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
-        <v>88</v>
+      <c r="A57" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C57" s="29" t="s">
         <v>48</v>
@@ -3549,7 +3528,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F57" s="32" t="s">
         <v>54</v>
@@ -3569,11 +3548,11 @@
       <c r="O57" s="16"/>
     </row>
     <row r="58" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="20" t="s">
-        <v>88</v>
+      <c r="A58" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C58" s="29" t="s">
         <v>48</v>
@@ -3582,7 +3561,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F58" s="32" t="s">
         <v>54</v>
@@ -3602,11 +3581,11 @@
       <c r="O58" s="16"/>
     </row>
     <row r="59" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
-        <v>88</v>
+      <c r="A59" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C59" s="29" t="s">
         <v>48</v>
@@ -3615,7 +3594,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F59" s="32" t="s">
         <v>54</v>
@@ -3652,11 +3631,11 @@
       <c r="O60" s="16"/>
     </row>
     <row r="61" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
-        <v>89</v>
+      <c r="A61" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C61" s="30" t="s">
         <v>48</v>
@@ -3665,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="F61" s="19" t="s">
         <v>55</v>
@@ -3690,11 +3669,11 @@
       <c r="Q61" s="18"/>
     </row>
     <row r="62" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
-        <v>89</v>
+      <c r="A62" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C62" s="29" t="s">
         <v>48</v>
@@ -3703,7 +3682,7 @@
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="F62" s="32" t="s">
         <v>55</v>
@@ -3724,11 +3703,11 @@
       <c r="Q62" s="18"/>
     </row>
     <row r="63" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>89</v>
+      <c r="A63" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C63" s="29" t="s">
         <v>48</v>
@@ -3737,7 +3716,7 @@
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="F63" s="32" t="s">
         <v>55</v>
@@ -3757,11 +3736,11 @@
       <c r="O63" s="16"/>
     </row>
     <row r="64" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
-        <v>89</v>
+      <c r="A64" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C64" s="29" t="s">
         <v>48</v>
@@ -3770,7 +3749,7 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="F64" s="32" t="s">
         <v>55</v>
@@ -3807,11 +3786,11 @@
       <c r="O65" s="16"/>
     </row>
     <row r="66" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
-        <v>90</v>
+      <c r="A66" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="B66" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C66" s="30" t="s">
         <v>48</v>
@@ -3820,7 +3799,7 @@
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="F66" s="19" t="s">
         <v>56</v>
@@ -3844,11 +3823,11 @@
       <c r="O66" s="16"/>
     </row>
     <row r="67" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
-        <v>90</v>
+      <c r="A67" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C67" s="29" t="s">
         <v>48</v>
@@ -3857,7 +3836,7 @@
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="F67" s="32" t="s">
         <v>56</v>
@@ -3877,11 +3856,11 @@
       <c r="O67" s="16"/>
     </row>
     <row r="68" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="20" t="s">
-        <v>90</v>
+      <c r="A68" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C68" s="29" t="s">
         <v>48</v>
@@ -3890,7 +3869,7 @@
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="F68" s="32" t="s">
         <v>56</v>
@@ -3910,11 +3889,11 @@
       <c r="O68" s="16"/>
     </row>
     <row r="69" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="20" t="s">
-        <v>90</v>
+      <c r="A69" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>48</v>
@@ -3923,7 +3902,7 @@
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="F69" s="32" t="s">
         <v>56</v>
@@ -3960,11 +3939,11 @@
       <c r="O70" s="16"/>
     </row>
     <row r="71" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
-        <v>91</v>
+      <c r="A71" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C71" s="30" t="s">
         <v>48</v>
@@ -3973,7 +3952,7 @@
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="F71" s="19" t="s">
         <v>57</v>
@@ -3997,11 +3976,11 @@
       <c r="O71" s="16"/>
     </row>
     <row r="72" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="20" t="s">
-        <v>91</v>
+      <c r="A72" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C72" s="29" t="s">
         <v>48</v>
@@ -4010,7 +3989,7 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="F72" s="32" t="s">
         <v>57</v>
@@ -4030,11 +4009,11 @@
       <c r="O72" s="16"/>
     </row>
     <row r="73" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
-        <v>91</v>
+      <c r="A73" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C73" s="29" t="s">
         <v>48</v>
@@ -4043,7 +4022,7 @@
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="F73" s="32" t="s">
         <v>57</v>
@@ -4063,11 +4042,11 @@
       <c r="O73" s="16"/>
     </row>
     <row r="74" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="20" t="s">
-        <v>91</v>
+      <c r="A74" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C74" s="29" t="s">
         <v>48</v>
@@ -4076,7 +4055,7 @@
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="F74" s="32" t="s">
         <v>57</v>
@@ -4113,11 +4092,11 @@
       <c r="O75" s="16"/>
     </row>
     <row r="76" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="18" t="s">
-        <v>92</v>
+      <c r="A76" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C76" s="30" t="s">
         <v>48</v>
@@ -4126,7 +4105,7 @@
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F76" s="19" t="s">
         <v>58</v>
@@ -4150,11 +4129,11 @@
       <c r="O76" s="16"/>
     </row>
     <row r="77" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="20" t="s">
-        <v>92</v>
+      <c r="A77" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C77" s="29" t="s">
         <v>48</v>
@@ -4163,7 +4142,7 @@
         <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F77" s="32" t="s">
         <v>58</v>
@@ -4183,11 +4162,11 @@
       <c r="O77" s="16"/>
     </row>
     <row r="78" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="20" t="s">
-        <v>92</v>
+      <c r="A78" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C78" s="29" t="s">
         <v>48</v>
@@ -4196,7 +4175,7 @@
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F78" s="32" t="s">
         <v>58</v>
@@ -4216,11 +4195,11 @@
       <c r="O78" s="16"/>
     </row>
     <row r="79" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="20" t="s">
-        <v>92</v>
+      <c r="A79" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C79" s="29" t="s">
         <v>48</v>
@@ -4229,7 +4208,7 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F79" s="32" t="s">
         <v>58</v>
@@ -4266,11 +4245,11 @@
       <c r="O80" s="16"/>
     </row>
     <row r="81" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
-        <v>95</v>
+      <c r="A81" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C81" s="30" t="s">
         <v>48</v>
@@ -4279,7 +4258,7 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F81" s="23" t="s">
         <v>59</v>
@@ -4287,7 +4266,7 @@
       <c r="G81" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H81" s="50">
+      <c r="H81" s="49">
         <v>5076</v>
       </c>
       <c r="I81" s="23" t="s">
@@ -4297,17 +4276,17 @@
         <v>748</v>
       </c>
       <c r="K81" s="24"/>
-      <c r="L81" s="23"/>
+      <c r="L81" s="19"/>
       <c r="M81" s="24"/>
       <c r="N81" s="24"/>
       <c r="O81" s="24"/>
     </row>
     <row r="82" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="25" t="s">
-        <v>95</v>
+      <c r="A82" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="B82" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C82" s="29" t="s">
         <v>48</v>
@@ -4316,7 +4295,7 @@
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F82" s="32" t="s">
         <v>59</v>
@@ -4336,11 +4315,11 @@
       <c r="O82" s="16"/>
     </row>
     <row r="83" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="s">
-        <v>95</v>
+      <c r="A83" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="B83" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C83" s="29" t="s">
         <v>48</v>
@@ -4349,7 +4328,7 @@
         <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F83" s="32" t="s">
         <v>59</v>
@@ -4369,11 +4348,11 @@
       <c r="O83" s="16"/>
     </row>
     <row r="84" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="25" t="s">
-        <v>95</v>
+      <c r="A84" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="B84" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C84" s="29" t="s">
         <v>48</v>
@@ -4382,7 +4361,7 @@
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F84" s="32" t="s">
         <v>59</v>
@@ -4419,11 +4398,11 @@
       <c r="O85" s="16"/>
     </row>
     <row r="86" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="18" t="s">
-        <v>94</v>
+      <c r="A86" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C86" s="30" t="s">
         <v>48</v>
@@ -4432,7 +4411,7 @@
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F86" s="19" t="s">
         <v>60</v>
@@ -4440,7 +4419,7 @@
       <c r="G86" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H86" s="50">
+      <c r="H86" s="49">
         <v>5076</v>
       </c>
       <c r="I86" s="17" t="s">
@@ -4456,11 +4435,11 @@
       <c r="O86" s="16"/>
     </row>
     <row r="87" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="20" t="s">
-        <v>94</v>
+      <c r="A87" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C87" s="29" t="s">
         <v>48</v>
@@ -4469,7 +4448,7 @@
         <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F87" s="32" t="s">
         <v>60</v>
@@ -4489,11 +4468,11 @@
       <c r="O87" s="16"/>
     </row>
     <row r="88" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="20" t="s">
-        <v>94</v>
+      <c r="A88" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C88" s="29" t="s">
         <v>48</v>
@@ -4502,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F88" s="32" t="s">
         <v>60</v>
@@ -4522,11 +4501,11 @@
       <c r="O88" s="16"/>
     </row>
     <row r="89" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="20" t="s">
-        <v>94</v>
+      <c r="A89" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C89" s="29" t="s">
         <v>48</v>
@@ -4535,7 +4514,7 @@
         <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F89" s="32" t="s">
         <v>60</v>
@@ -4572,11 +4551,11 @@
       <c r="O90" s="16"/>
     </row>
     <row r="91" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="18" t="s">
-        <v>93</v>
+      <c r="A91" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C91" s="30" t="s">
         <v>48</v>
@@ -4585,7 +4564,7 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F91" s="19" t="s">
         <v>61</v>
@@ -4593,7 +4572,7 @@
       <c r="G91" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H91" s="50">
+      <c r="H91" s="49">
         <v>5076</v>
       </c>
       <c r="I91" s="17" t="s">
@@ -4609,11 +4588,11 @@
       <c r="O91" s="16"/>
     </row>
     <row r="92" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="20" t="s">
-        <v>93</v>
+      <c r="A92" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C92" s="29" t="s">
         <v>48</v>
@@ -4622,7 +4601,7 @@
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F92" s="32" t="s">
         <v>61</v>
@@ -4642,11 +4621,11 @@
       <c r="O92" s="16"/>
     </row>
     <row r="93" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="20" t="s">
-        <v>93</v>
+      <c r="A93" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C93" s="29" t="s">
         <v>48</v>
@@ -4655,7 +4634,7 @@
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F93" s="32" t="s">
         <v>61</v>
@@ -4675,11 +4654,11 @@
       <c r="O93" s="16"/>
     </row>
     <row r="94" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="20" t="s">
-        <v>93</v>
+      <c r="A94" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C94" s="29" t="s">
         <v>48</v>
@@ -4688,7 +4667,7 @@
         <v>2</v>
       </c>
       <c r="E94" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F94" s="32" t="s">
         <v>61</v>
@@ -4726,10 +4705,10 @@
     </row>
     <row r="96" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="16" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B96" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C96" s="30" t="s">
         <v>48</v>
@@ -4738,7 +4717,7 @@
         <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F96" s="23" t="s">
         <v>62</v>
@@ -4746,7 +4725,7 @@
       <c r="G96" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H96" s="50">
+      <c r="H96" s="49">
         <v>5076</v>
       </c>
       <c r="I96" s="23" t="s">
@@ -4756,17 +4735,17 @@
         <v>1806</v>
       </c>
       <c r="K96" s="24"/>
-      <c r="L96" s="23"/>
+      <c r="L96" s="19"/>
       <c r="M96" s="24"/>
       <c r="N96" s="24"/>
       <c r="O96" s="24"/>
     </row>
     <row r="97" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="25" t="s">
-        <v>96</v>
+      <c r="A97" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="B97" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C97" s="29" t="s">
         <v>48</v>
@@ -4775,7 +4754,7 @@
         <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F97" s="32" t="s">
         <v>62</v>
@@ -4795,11 +4774,11 @@
       <c r="O97" s="16"/>
     </row>
     <row r="98" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="25" t="s">
-        <v>96</v>
+      <c r="A98" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="B98" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C98" s="29" t="s">
         <v>48</v>
@@ -4808,7 +4787,7 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F98" s="32" t="s">
         <v>62</v>
@@ -4846,10 +4825,10 @@
     </row>
     <row r="100" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="16" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C100" s="30" t="s">
         <v>48</v>
@@ -4858,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F100" s="19" t="s">
         <v>63</v>
@@ -4866,7 +4845,7 @@
       <c r="G100" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H100" s="50">
+      <c r="H100" s="49">
         <v>5076</v>
       </c>
       <c r="I100" s="17" t="s">
@@ -4882,11 +4861,11 @@
       <c r="O100" s="16"/>
     </row>
     <row r="101" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="20" t="s">
-        <v>97</v>
+      <c r="A101" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="B101" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C101" s="29" t="s">
         <v>48</v>
@@ -4895,7 +4874,7 @@
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F101" s="32" t="s">
         <v>63</v>
@@ -4915,11 +4894,11 @@
       <c r="O101" s="16"/>
     </row>
     <row r="102" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="20" t="s">
-        <v>97</v>
+      <c r="A102" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C102" s="29" t="s">
         <v>48</v>
@@ -4928,7 +4907,7 @@
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F102" s="32" t="s">
         <v>63</v>
@@ -4966,10 +4945,10 @@
     </row>
     <row r="104" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="16" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C104" s="30" t="s">
         <v>48</v>
@@ -4978,7 +4957,7 @@
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="F104" s="19" t="s">
         <v>64</v>
@@ -4986,7 +4965,7 @@
       <c r="G104" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H104" s="50">
+      <c r="H104" s="49">
         <v>5076</v>
       </c>
       <c r="I104" s="17" t="s">
@@ -5002,11 +4981,11 @@
       <c r="O104" s="16"/>
     </row>
     <row r="105" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="20" t="s">
-        <v>98</v>
+      <c r="A105" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="B105" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C105" s="29" t="s">
         <v>48</v>
@@ -5015,7 +4994,7 @@
         <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="F105" s="32" t="s">
         <v>64</v>
@@ -5035,11 +5014,11 @@
       <c r="O105" s="16"/>
     </row>
     <row r="106" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="20" t="s">
-        <v>98</v>
+      <c r="A106" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C106" s="29" t="s">
         <v>48</v>
@@ -5048,7 +5027,7 @@
         <v>2</v>
       </c>
       <c r="E106" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="F106" s="32" t="s">
         <v>64</v>
@@ -5085,11 +5064,11 @@
       <c r="O107" s="16"/>
     </row>
     <row r="108" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>99</v>
+      <c r="A108" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C108" s="30" t="s">
         <v>48</v>
@@ -5098,7 +5077,7 @@
         <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="F108" s="19" t="s">
         <v>65</v>
@@ -5106,7 +5085,7 @@
       <c r="G108" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H108" s="50">
+      <c r="H108" s="49">
         <v>5076</v>
       </c>
       <c r="I108" s="17" t="s">
@@ -5122,11 +5101,11 @@
       <c r="O108" s="16"/>
     </row>
     <row r="109" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="20" t="s">
-        <v>99</v>
+      <c r="A109" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="B109" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C109" s="29" t="s">
         <v>48</v>
@@ -5135,7 +5114,7 @@
         <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="F109" s="32" t="s">
         <v>65</v>
@@ -5155,11 +5134,11 @@
       <c r="O109" s="16"/>
     </row>
     <row r="110" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="20" t="s">
-        <v>99</v>
+      <c r="A110" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="B110" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C110" s="29" t="s">
         <v>48</v>
@@ -5168,7 +5147,7 @@
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="F110" s="32" t="s">
         <v>65</v>
@@ -5194,13 +5173,14 @@
       <c r="D111" s="31"/>
       <c r="E111" s="31"/>
       <c r="I111" s="2"/>
+      <c r="L111" s="19"/>
     </row>
     <row r="112" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>100</v>
+      <c r="A112" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C112" s="30" t="s">
         <v>48</v>
@@ -5209,7 +5189,7 @@
         <v>2</v>
       </c>
       <c r="E112" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>66</v>
@@ -5226,13 +5206,14 @@
       <c r="J112" s="19">
         <v>1805</v>
       </c>
+      <c r="L112" s="19"/>
     </row>
     <row r="113" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="20" t="s">
-        <v>100</v>
+      <c r="A113" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C113" s="29" t="s">
         <v>48</v>
@@ -5241,7 +5222,7 @@
         <v>2</v>
       </c>
       <c r="E113" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="F113" s="31" t="s">
         <v>66</v>
@@ -5253,6 +5234,7 @@
         <v>-39.353616666666667</v>
       </c>
       <c r="I113" s="2"/>
+      <c r="L113" s="19"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="20"/>
@@ -5272,11 +5254,11 @@
       <c r="O114" s="16"/>
     </row>
     <row r="115" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>101</v>
+      <c r="A115" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="B115" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C115" s="30" t="s">
         <v>48</v>
@@ -5285,7 +5267,7 @@
         <v>2</v>
       </c>
       <c r="E115" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>67</v>
@@ -5302,13 +5284,14 @@
       <c r="J115" s="19">
         <v>2108</v>
       </c>
+      <c r="L115" s="19"/>
     </row>
     <row r="116" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="20" t="s">
-        <v>101</v>
+      <c r="A116" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="B116" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C116" s="29" t="s">
         <v>48</v>
@@ -5317,7 +5300,7 @@
         <v>2</v>
       </c>
       <c r="E116" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="F116" s="31" t="s">
         <v>67</v>
@@ -5329,6 +5312,7 @@
         <v>-39.353616666666667</v>
       </c>
       <c r="I116" s="2"/>
+      <c r="L116" s="19"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="20"/>
@@ -5348,20 +5332,20 @@
       <c r="O117" s="16"/>
     </row>
     <row r="118" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>102</v>
+      <c r="A118" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="B118" t="s">
+        <v>83</v>
+      </c>
+      <c r="C118" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D118" s="8">
+        <v>2</v>
+      </c>
+      <c r="E118" t="s">
         <v>106</v>
-      </c>
-      <c r="C118" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D118" s="8">
-        <v>2</v>
-      </c>
-      <c r="E118" t="s">
-        <v>129</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>68</v>
@@ -5378,22 +5362,23 @@
       <c r="J118" s="19">
         <v>2409</v>
       </c>
+      <c r="L118" s="19"/>
     </row>
     <row r="119" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="20" t="s">
-        <v>102</v>
+      <c r="A119" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="B119" t="s">
+        <v>83</v>
+      </c>
+      <c r="C119" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D119" s="31">
+        <v>2</v>
+      </c>
+      <c r="E119" t="s">
         <v>106</v>
-      </c>
-      <c r="C119" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D119" s="31">
-        <v>2</v>
-      </c>
-      <c r="E119" t="s">
-        <v>129</v>
       </c>
       <c r="F119" s="31" t="s">
         <v>68</v>
@@ -5405,6 +5390,7 @@
         <v>-39.353616666666667</v>
       </c>
       <c r="I119" s="2"/>
+      <c r="L119" s="19"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="20"/>
@@ -5424,11 +5410,11 @@
       <c r="O120" s="16"/>
     </row>
     <row r="121" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>103</v>
+      <c r="A121" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C121" s="30" t="s">
         <v>48</v>
@@ -5437,7 +5423,7 @@
         <v>2</v>
       </c>
       <c r="E121" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>69</v>
@@ -5454,13 +5440,14 @@
       <c r="J121" s="19">
         <v>2709</v>
       </c>
+      <c r="L121" s="19"/>
     </row>
     <row r="122" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="20" t="s">
-        <v>103</v>
+      <c r="A122" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="B122" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C122" s="29" t="s">
         <v>48</v>
@@ -5469,7 +5456,7 @@
         <v>2</v>
       </c>
       <c r="E122" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F122" s="31" t="s">
         <v>69</v>
@@ -5481,6 +5468,7 @@
         <v>-39.353616666666667</v>
       </c>
       <c r="I122" s="2"/>
+      <c r="L122" s="19"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="20"/>
@@ -5501,10 +5489,10 @@
     </row>
     <row r="124" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B124" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C124" s="30" t="s">
         <v>48</v>
@@ -5513,9 +5501,9 @@
         <v>2</v>
       </c>
       <c r="E124" t="s">
-        <v>133</v>
-      </c>
-      <c r="F124" s="49">
+        <v>110</v>
+      </c>
+      <c r="F124" s="48">
         <v>14874</v>
       </c>
       <c r="G124" s="6"/>
@@ -5532,13 +5520,14 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I125" s="2"/>
+      <c r="L125" s="19"/>
     </row>
     <row r="126" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="B126" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C126" s="47" t="s">
         <v>48</v>
@@ -5547,7 +5536,7 @@
         <v>2</v>
       </c>
       <c r="E126" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="F126" s="46">
         <v>14876</v>
@@ -5559,7 +5548,7 @@
       </c>
       <c r="J126" s="46"/>
       <c r="K126" s="46"/>
-      <c r="L126" s="48"/>
+      <c r="L126" s="19"/>
       <c r="M126" s="46"/>
       <c r="N126" s="46"/>
       <c r="O126" s="46"/>
@@ -5634,7 +5623,6 @@
       <c r="C131" s="16"/>
       <c r="D131" s="17"/>
       <c r="E131" s="17"/>
-      <c r="F131" s="16"/>
       <c r="H131" s="16"/>
       <c r="I131" s="17"/>
       <c r="J131" s="16"/>
@@ -5644,6 +5632,15 @@
       <c r="N131" s="16"/>
       <c r="O131" s="16"/>
     </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F132" s="16"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F133" s="16"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F134" s="16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>